<commit_message>
updated clean stat files
</commit_message>
<xml_diff>
--- a/KAT2324.xlsx
+++ b/KAT2324.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FFE8FDD-E325-42A5-8D08-D350416D011B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17A6F91D-887E-4855-A33C-B7BEE2D6BECB}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,7 +635,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -976,7 +976,7 @@
   <dimension ref="A1:AD83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1167,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
         <v>45227</v>
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>45229</v>
@@ -1348,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
         <v>45231</v>
@@ -1437,7 +1437,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>45234</v>
@@ -1526,7 +1526,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <v>45236</v>
@@ -1612,7 +1612,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <v>45238</v>
@@ -1701,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2">
         <v>45240</v>
@@ -1793,7 +1793,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
         <v>45242</v>
@@ -1885,7 +1885,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
         <v>45244</v>
@@ -1977,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>45245</v>
@@ -2069,7 +2069,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2">
         <v>45248</v>
@@ -2161,7 +2161,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2">
         <v>45250</v>
@@ -2250,7 +2250,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>45252</v>
@@ -2339,7 +2339,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2">
         <v>45254</v>
@@ -2428,7 +2428,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2">
         <v>45256</v>
@@ -2520,7 +2520,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2">
         <v>45258</v>
@@ -2609,7 +2609,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
         <v>45260</v>
@@ -2698,7 +2698,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2">
         <v>45262</v>
@@ -2787,7 +2787,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2">
         <v>45266</v>
@@ -2876,7 +2876,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2">
         <v>45268</v>
@@ -2968,7 +2968,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2">
         <v>45271</v>
@@ -3060,7 +3060,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2">
         <v>45274</v>
@@ -3152,7 +3152,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C25" s="2">
         <v>45276</v>
@@ -3241,7 +3241,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2">
         <v>45278</v>
@@ -3333,7 +3333,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
         <v>45280</v>
@@ -3425,7 +3425,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2">
         <v>45281</v>
@@ -3513,6 +3513,9 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
+      <c r="B29">
+        <v>32</v>
+      </c>
       <c r="C29" s="2">
         <v>45283</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2">
         <v>45286</v>
@@ -3695,7 +3698,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
         <v>45288</v>
@@ -3784,7 +3787,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2">
         <v>45290</v>
@@ -3873,7 +3876,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2">
         <v>45292</v>
@@ -4054,7 +4057,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="2">
         <v>45296</v>
@@ -4146,7 +4149,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2">
         <v>45298</v>
@@ -4238,7 +4241,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2">
         <v>45300</v>
@@ -4330,7 +4333,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C38" s="2">
         <v>45301</v>
@@ -4422,7 +4425,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2">
         <v>45303</v>
@@ -4511,7 +4514,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C40" s="2">
         <v>45305</v>
@@ -4600,7 +4603,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C41" s="2">
         <v>45308</v>
@@ -4692,7 +4695,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C42" s="2">
         <v>45309</v>
@@ -4781,7 +4784,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C43" s="2">
         <v>45311</v>
@@ -4870,7 +4873,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C44" s="2">
         <v>45313</v>
@@ -4959,7 +4962,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C45" s="2">
         <v>45315</v>
@@ -5051,7 +5054,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C46" s="2">
         <v>45316</v>
@@ -5143,7 +5146,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C47" s="2">
         <v>45318</v>
@@ -5235,7 +5238,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C48" s="2">
         <v>45320</v>
@@ -5327,7 +5330,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C49" s="2">
         <v>45322</v>
@@ -5416,7 +5419,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C50" s="2">
         <v>45324</v>
@@ -5505,7 +5508,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C51" s="2">
         <v>45326</v>
@@ -5594,7 +5597,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C52" s="2">
         <v>45328</v>
@@ -5686,7 +5689,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C53" s="2">
         <v>45330</v>
@@ -5778,7 +5781,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2">
         <v>45334</v>
@@ -5870,7 +5873,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C55" s="2">
         <v>45335</v>
@@ -5962,7 +5965,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C56" s="2">
         <v>45337</v>
@@ -6054,7 +6057,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C57" s="2">
         <v>45345</v>
@@ -6143,7 +6146,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C58" s="2">
         <v>45346</v>
@@ -6231,6 +6234,9 @@
       <c r="A59" s="1">
         <v>58</v>
       </c>
+      <c r="B59">
+        <v>32</v>
+      </c>
       <c r="C59" s="2">
         <v>45349</v>
       </c>
@@ -6318,7 +6324,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C60" s="2">
         <v>45350</v>
@@ -6404,7 +6410,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C61" s="2">
         <v>45352</v>
@@ -6493,7 +6499,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C62" s="2">
         <v>45354</v>
@@ -6582,7 +6588,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C63" s="2">
         <v>45355</v>
@@ -6670,6 +6676,9 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
+      <c r="B64">
+        <v>32</v>
+      </c>
       <c r="C64" s="2">
         <v>45358</v>
       </c>
@@ -6759,6 +6768,9 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
+      <c r="B65">
+        <v>32</v>
+      </c>
       <c r="C65" s="2">
         <v>45359</v>
       </c>
@@ -6848,6 +6860,9 @@
       <c r="A66" s="1">
         <v>65</v>
       </c>
+      <c r="B66">
+        <v>32</v>
+      </c>
       <c r="C66" s="2">
         <v>45361</v>
       </c>
@@ -6937,6 +6952,9 @@
       <c r="A67" s="1">
         <v>66</v>
       </c>
+      <c r="B67">
+        <v>32</v>
+      </c>
       <c r="C67" s="2">
         <v>45363</v>
       </c>
@@ -7026,6 +7044,9 @@
       <c r="A68" s="1">
         <v>67</v>
       </c>
+      <c r="B68">
+        <v>32</v>
+      </c>
       <c r="C68" s="2">
         <v>45367</v>
       </c>
@@ -7115,6 +7136,9 @@
       <c r="A69" s="1">
         <v>68</v>
       </c>
+      <c r="B69">
+        <v>32</v>
+      </c>
       <c r="C69" s="2">
         <v>45369</v>
       </c>
@@ -7204,6 +7228,9 @@
       <c r="A70" s="1">
         <v>69</v>
       </c>
+      <c r="B70">
+        <v>32</v>
+      </c>
       <c r="C70" s="2">
         <v>45370</v>
       </c>
@@ -7290,6 +7317,9 @@
       <c r="A71" s="1">
         <v>70</v>
       </c>
+      <c r="B71">
+        <v>32</v>
+      </c>
       <c r="C71" s="2">
         <v>45373</v>
       </c>
@@ -7376,6 +7406,9 @@
       <c r="A72" s="1">
         <v>71</v>
       </c>
+      <c r="B72">
+        <v>32</v>
+      </c>
       <c r="C72" s="2">
         <v>45375</v>
       </c>
@@ -7462,6 +7495,9 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
+      <c r="B73">
+        <v>32</v>
+      </c>
       <c r="C73" s="2">
         <v>45378</v>
       </c>
@@ -7548,6 +7584,9 @@
       <c r="A74" s="1">
         <v>73</v>
       </c>
+      <c r="B74">
+        <v>32</v>
+      </c>
       <c r="C74" s="2">
         <v>45380</v>
       </c>
@@ -7637,6 +7676,9 @@
       <c r="A75" s="1">
         <v>74</v>
       </c>
+      <c r="B75">
+        <v>32</v>
+      </c>
       <c r="C75" s="2">
         <v>45382</v>
       </c>
@@ -7723,6 +7765,9 @@
       <c r="A76" s="1">
         <v>75</v>
       </c>
+      <c r="B76">
+        <v>32</v>
+      </c>
       <c r="C76" s="2">
         <v>45384</v>
       </c>
@@ -7809,6 +7854,9 @@
       <c r="A77" s="1">
         <v>76</v>
       </c>
+      <c r="B77">
+        <v>32</v>
+      </c>
       <c r="C77" s="2">
         <v>45385</v>
       </c>
@@ -7895,6 +7943,9 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
+      <c r="B78">
+        <v>32</v>
+      </c>
       <c r="C78" s="2">
         <v>45387</v>
       </c>
@@ -7984,6 +8035,9 @@
       <c r="A79" s="1">
         <v>78</v>
       </c>
+      <c r="B79">
+        <v>32</v>
+      </c>
       <c r="C79" s="2">
         <v>45389</v>
       </c>
@@ -8073,6 +8127,9 @@
       <c r="A80" s="1">
         <v>79</v>
       </c>
+      <c r="B80">
+        <v>32</v>
+      </c>
       <c r="C80" s="2">
         <v>45391</v>
       </c>
@@ -8159,6 +8216,9 @@
       <c r="A81" s="1">
         <v>80</v>
       </c>
+      <c r="B81">
+        <v>32</v>
+      </c>
       <c r="C81" s="2">
         <v>45392</v>
       </c>
@@ -8249,7 +8309,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C82" s="2">
         <v>45394</v>
@@ -8338,7 +8398,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C83" s="2">
         <v>45396</v>

</xml_diff>